<commit_message>
add ecosystem overfishing, fix engagement, fix aqua
</commit_message>
<xml_diff>
--- a/data-raw/SocVul_in_Top_Fishing_Communities_120820_WENG - Changhua Weng - NOAA Affiliate.xlsx
+++ b/data-raw/SocVul_in_Top_Fishing_Communities_120820_WENG - Changhua Weng - NOAA Affiliate.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\changhua.weng\Documents\a Social Indicators\SOE Report\2021 Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kimberly.bastille\Desktop\Rgghhh\ecodata\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="649" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="649"/>
   </bookViews>
   <sheets>
     <sheet name="Top 10 Communities_Mid-Atlantic" sheetId="24" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="78">
   <si>
     <t>STATEABBR</t>
   </si>
@@ -157,9 +157,6 @@
   </si>
   <si>
     <t>Cape May, NJ</t>
-  </si>
-  <si>
-    <t>Point Pleasant, NJ</t>
   </si>
   <si>
     <t>Point Pleasant Beach, NJ</t>
@@ -620,7 +617,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -681,13 +677,12 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7EEE9CA-334C-480D-8F47-B4AF27CB66FC}" type="CELLRANGE">
+                    <a:fld id="{AEA9EDF3-85C9-432E-BB2B-06E50739B4B3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -705,7 +700,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -717,13 +711,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6C17B06F-A61F-4BBD-B40C-4ACF003F4889}" type="CELLRANGE">
+                    <a:fld id="{2CF211E1-5BAB-4421-8B47-86CD03408C6C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -741,7 +734,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -764,7 +756,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{821FBA2D-0BD6-4D8F-95F6-A89114A530C7}" type="CELLRANGE">
+                    <a:fld id="{F1E2FE2A-D8C9-499A-BE94-305D409060DE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -782,7 +774,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -804,7 +795,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DF2CD4E0-EF93-4613-ADE1-3B45DD56394C}" type="CELLRANGE">
+                    <a:fld id="{FE798BB0-C837-4B26-A915-E57B979D7524}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -822,7 +813,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -833,13 +823,12 @@
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
-              <c:layout/>
               <c:tx>
                 <c:rich>
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0362304C-1405-4A0C-B0FA-0392F37A4ACB}" type="CELLRANGE">
+                    <a:fld id="{235C941B-7DF9-413F-8980-8899B73E9EC1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -857,7 +846,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
@@ -901,7 +889,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -1059,7 +1046,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{20B172E4-4487-4BE0-9D14-01415FFE52E3}" type="CELLRANGE">
+                    <a:fld id="{09225D20-4402-4CC7-8F28-CC4C28C9C6FF}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1076,7 +1063,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1098,7 +1084,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D582485-0F0D-40B6-9DF1-1739A0F18233}" type="CELLRANGE">
+                    <a:fld id="{7E90CF3D-496C-44A2-BECC-B7F6184FA280}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1115,7 +1101,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1137,7 +1122,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4A65560A-D4D6-4E0A-99CC-6AB7B0AE263C}" type="CELLRANGE">
+                    <a:fld id="{2E270616-BBE7-493B-8700-434DA6EC4E72}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1154,7 +1139,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1176,7 +1160,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{035DF2B5-843A-4265-ADF4-19310E427B50}" type="CELLRANGE">
+                    <a:fld id="{92FEAC11-C642-4F7F-8512-9F7C61DDC201}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1193,7 +1177,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1215,7 +1198,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FEA365B9-EB2E-4BB9-A6A6-2F9503F1E6CD}" type="CELLRANGE">
+                    <a:fld id="{1C1C9A1D-4E92-4134-A973-B21888F7A123}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1232,7 +1215,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1254,7 +1236,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{512460CC-F4DA-48EF-A7A3-5C271DE964C1}" type="CELLRANGE">
+                    <a:fld id="{15E8610B-7528-4639-9559-0933AF2B0ED7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1271,7 +1253,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -1293,7 +1274,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A7E4272E-4FD0-4BE7-BB97-96180A75B223}" type="CELLRANGE">
+                    <a:fld id="{DE6CA66E-7B19-437D-914A-29997D1A1F47}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1310,7 +1291,6 @@
               <c:showBubbleSize val="0"/>
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
                   <c15:dlblFieldTable/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
@@ -2131,7 +2111,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{983D49A7-7121-4AE1-AC7B-BCF96A7ECDF5}" type="CELLRANGE">
+                    <a:fld id="{5C3719DC-B413-4058-9598-3AE272420998}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2166,7 +2146,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EEBDAE36-1DC6-4C5F-9D31-0A69557AE2F6}" type="CELLRANGE">
+                    <a:fld id="{B63611E9-CE18-4296-A6BD-D5DEADD0730E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2206,7 +2186,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A73FBF2-4626-4411-919D-81DDE908FD4B}" type="CELLRANGE">
+                    <a:fld id="{FDFBD74C-2FE4-4DF9-BE34-ACDAE8E0312E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2240,7 +2220,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{886C498C-CADB-487B-9E49-04FB63871247}" type="CELLRANGE">
+                    <a:fld id="{535AE70D-E2B4-4930-886C-8B4A53D9D0D1}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2466,7 +2446,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DE086736-FA65-4460-8DC5-11B86EE242D5}" type="CELLRANGE">
+                    <a:fld id="{947B19CA-815B-4EAF-B7BB-78B51AD8C12A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2505,7 +2485,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{35D9B453-B9E3-4921-A42C-5DF19B98828B}" type="CELLRANGE">
+                    <a:fld id="{47FCF38C-CB76-4F16-AB28-A816CFBCE1D4}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2539,7 +2519,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC0EF8C1-2438-4445-9DE8-EAE7829F0BE5}" type="CELLRANGE">
+                    <a:fld id="{51BC5FB7-D3C7-4EDE-88F6-755ABE10FFD5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2579,7 +2559,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9A52BA48-3B74-4EE6-A1B7-7B8B5EBE1A20}" type="CELLRANGE">
+                    <a:fld id="{239BE61E-E98B-4C9C-A169-384D606C7100}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2618,7 +2598,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C737D995-2283-4E7E-904D-4FC4A6253B1E}" type="CELLRANGE">
+                    <a:fld id="{DADF5907-1422-4BF8-AD95-9AC0323E9BD5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2657,7 +2637,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D900ED13-56FE-4F1F-8CA2-923FDDBFCED1}" type="CELLRANGE">
+                    <a:fld id="{1C3EFAD8-9868-4409-8EEF-7F8C8B9273CA}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2696,7 +2676,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BF03938F-3873-4CCB-A479-57D35FB4A017}" type="CELLRANGE">
+                    <a:fld id="{2DF4CC9D-B4CC-481F-9832-EDEBB9DA30E0}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2735,7 +2715,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4024CDB9-FAE5-4236-950E-464CBB5BA7EC}" type="CELLRANGE">
+                    <a:fld id="{F9E9F6EE-4BF8-4CED-8D1B-8A027C070ACE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2774,7 +2754,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F46D5676-0A2B-4BA1-9656-9E958745F18B}" type="CELLRANGE">
+                    <a:fld id="{61EDFADD-8AAA-4D0E-A8E0-D44B1CEC9BCE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2813,7 +2793,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AB96F8B1-BEA0-4796-B4CE-B0EA414D5C86}" type="CELLRANGE">
+                    <a:fld id="{CB5E1F4A-09F6-46A7-94B7-A0ED2543EA49}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2852,7 +2832,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A4D2BD9C-E13E-45C6-BAC2-A0175AC8A816}" type="CELLRANGE">
+                    <a:fld id="{435431A3-2549-430F-8E81-669864AEE43E}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2886,7 +2866,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7DDDCF0B-6549-4701-B9D6-EA41F8AF7F13}" type="CELLRANGE">
+                    <a:fld id="{1E7A6F0B-C482-4928-BA54-D1A4A67067EE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -2926,7 +2906,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{92E41129-9D25-4D2D-B40A-1A00DF5C4A87}" type="CELLRANGE">
+                    <a:fld id="{2E613855-4849-4FC9-9DED-622A31C5F730}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3194,7 +3174,7 @@
                     <c:v>Nags Head, NC</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>Point Pleasant, NJ</c:v>
+                    <c:v>Point Pleasant Beach, NJ</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -3730,7 +3710,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{97546153-8F4D-4D20-ADAB-FE16C35E4442}" type="CELLRANGE">
+                    <a:fld id="{B598D708-D55D-43C1-A644-9C21925249A2}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3769,7 +3749,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6AD3F22E-FA24-4395-906E-2E4DFAA1246F}" type="CELLRANGE">
+                    <a:fld id="{A63E8B31-F18F-499B-8721-8EBF1F149C06}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3808,7 +3788,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1E2D0929-B923-4580-962E-BEB38D9E28A1}" type="CELLRANGE">
+                    <a:fld id="{8DC7C9B2-F739-4C56-8F1B-29F7FC90E202}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4026,7 +4006,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EFB76148-74F0-4046-809B-1285754D7838}" type="CELLRANGE">
+                    <a:fld id="{8B1D5243-5D9F-4B21-9834-8B34813D5989}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4065,7 +4045,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A128F251-092E-4165-BAF1-5373E72C78A5}" type="CELLRANGE">
+                    <a:fld id="{3FD72705-9E8A-4155-BEC3-CC0C3D3C4B15}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4104,7 +4084,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3CDCE9E-3990-4D63-AF51-D8DB76E3CA98}" type="CELLRANGE">
+                    <a:fld id="{844E28D6-B3B0-4024-8B8D-A2FA61191DA5}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4143,7 +4123,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{87810C57-EFAD-442D-915F-93F78515BB88}" type="CELLRANGE">
+                    <a:fld id="{6FBF72DC-62D0-4CDB-97C4-125A4E35E4BC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4278,7 +4258,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2E851F52-F521-474F-BD75-3B4AFFD38B81}" type="CELLRANGE">
+                    <a:fld id="{035A00A1-E091-4437-B483-BB4254A0709F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4413,7 +4393,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{69CBF497-7A0D-4BCD-B746-A10D6F3878AB}" type="CELLRANGE">
+                    <a:fld id="{DD86C0FD-AF19-4EF8-ACC6-01C58DFABA07}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4457,7 +4437,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{03563A16-CEF7-40C1-9B6A-42EFD760496C}" type="CELLRANGE">
+                    <a:fld id="{189749CB-D457-44E1-A591-4381529383C3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4496,7 +4476,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A9BE7CD4-A31B-479F-856C-E5F0D0C3EDA4}" type="CELLRANGE">
+                    <a:fld id="{DCF766CE-6174-4619-B0BC-806A7FEA216B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4535,7 +4515,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E87287F7-C82C-4FD0-BC8C-01EEC613E31C}" type="CELLRANGE">
+                    <a:fld id="{0B77620E-C421-4510-B686-ABCFA411C8EE}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4574,7 +4554,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9FF713E9-E132-43F2-9C73-987CBDE8BC90}" type="CELLRANGE">
+                    <a:fld id="{630D3E44-1A15-4EC8-8019-22D6CB43FA60}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4613,7 +4593,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{23D26ED0-C849-41DB-A0DD-AF0BA0EDAEA9}" type="CELLRANGE">
+                    <a:fld id="{7D209E57-E7AD-4546-8AA6-66EA9B744045}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4647,7 +4627,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D1E02026-5F08-48EA-960C-313FCC4588B2}" type="CELLRANGE">
+                    <a:fld id="{1A909E6F-024E-45B7-BEE0-AC3234B91E1C}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5441,7 +5421,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3DCC64E7-443E-4D1D-A011-CCC510F88554}" type="CELLRANGE">
+                    <a:fld id="{059859CC-F46E-4275-8EE3-4FFB0CAD3A5F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5633,7 +5613,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{06F9D243-5D03-4404-A1C6-EBE898A9242D}" type="CELLRANGE">
+                    <a:fld id="{F48E3509-F8CE-4836-934F-9B4596A2E739}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5673,7 +5653,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1505EB70-B31B-44DB-8CF9-3CFB2A378542}" type="CELLRANGE">
+                    <a:fld id="{5B814DAF-3ECF-4296-8B2F-E0D3B3F38B76}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5812,7 +5792,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D081A7DC-9D52-4D17-BC6C-24198D11B5EC}" type="CELLRANGE">
+                    <a:fld id="{C00F6AC8-C356-4033-AD08-53A9FB2B26D7}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5851,7 +5831,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BE532330-DF50-4B75-96D1-9023531A03A4}" type="CELLRANGE">
+                    <a:fld id="{ACA66AEA-B596-43B8-A22F-2BE2C5CAC79F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5890,7 +5870,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E6B065B2-7FBD-47C8-9ECB-3E4D0B4EF8C2}" type="CELLRANGE">
+                    <a:fld id="{3C5E97C1-039D-43D5-B406-9BC78620B293}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5929,7 +5909,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{835A2790-103B-46EF-ACB5-2B50E32AA96B}" type="CELLRANGE">
+                    <a:fld id="{A354634E-EEE0-4D79-9CA4-7026E32BA719}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5968,7 +5948,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A2F63A15-41E1-4630-96DE-A321F62F08F6}" type="CELLRANGE">
+                    <a:fld id="{92C9DB1B-9FE1-46F9-943F-F6FFE156939F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6007,7 +5987,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A04C387F-325C-45B4-A950-1B6A7B15BC33}" type="CELLRANGE">
+                    <a:fld id="{A91DDF7C-2DDA-46D9-BED8-C1B475402B98}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6046,7 +6026,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B512457E-3817-496A-AD6A-EFDCCF0089E9}" type="CELLRANGE">
+                    <a:fld id="{2E8D0DC1-0804-48A9-AB36-71F3BD45BC27}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6085,7 +6065,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B29FF011-A4F4-46A3-8BA4-519BAE768CF2}" type="CELLRANGE">
+                    <a:fld id="{F2EA9664-94B8-4E6D-A393-A256502B0B21}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6124,7 +6104,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ED355EFC-248B-409A-97D4-36E038770816}" type="CELLRANGE">
+                    <a:fld id="{BD963654-0911-492C-9AEA-413E02EEF15F}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -6163,7 +6143,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DFC053FD-3D03-4B23-8735-CC4124C54ECD}" type="CELLRANGE">
+                    <a:fld id="{C2D98C08-044B-46AD-BD82-6DADE8799877}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -9482,8 +9462,713 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="2" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="9">
+        <v>6.9089999999999998</v>
+      </c>
+      <c r="E3" s="10">
+        <v>3.8239999999999998</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="9">
+        <v>3.8069999999999999</v>
+      </c>
+      <c r="E4" s="10">
+        <v>5.0570000000000004</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="9">
+        <v>2.0910000000000002</v>
+      </c>
+      <c r="E5" s="10">
+        <v>-4.2999999999999997E-2</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.217</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0.496</v>
+      </c>
+      <c r="F6" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.08</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1.7150000000000001</v>
+      </c>
+      <c r="F7" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="13">
+        <v>11.439</v>
+      </c>
+      <c r="E8" s="14">
+        <v>1.946</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="13">
+        <v>2.5779999999999998</v>
+      </c>
+      <c r="E9" s="14">
+        <v>-0.08</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="13">
+        <v>1.9790000000000001</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="13">
+        <v>1.6990000000000001</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0.625</v>
+      </c>
+      <c r="F11" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="13">
+        <v>-4.2999999999999997E-2</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="13">
+        <v>5.6289999999999996</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0.67200000000000004</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="13">
+        <v>4.8849999999999998</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="27">
+        <v>2.0409999999999999</v>
+      </c>
+      <c r="E15" s="26">
+        <v>-0.01</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="10">
+        <v>1.5409999999999999</v>
+      </c>
+      <c r="E36" s="10">
+        <v>5.1840000000000002</v>
+      </c>
+      <c r="F36" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" s="10">
+        <v>5.2190000000000003</v>
+      </c>
+      <c r="E37" s="10">
+        <v>15.752000000000001</v>
+      </c>
+      <c r="F37" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="10">
+        <v>0.51100000000000001</v>
+      </c>
+      <c r="E38" s="10">
+        <v>3.339</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" s="10">
+        <v>1.542</v>
+      </c>
+      <c r="E39" s="10">
+        <v>5.8360000000000003</v>
+      </c>
+      <c r="F39" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="14">
+        <v>2.097</v>
+      </c>
+      <c r="E40" s="14">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D41" s="14">
+        <v>6.3730000000000002</v>
+      </c>
+      <c r="E41" s="14">
+        <v>1.292</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="D42" s="14">
+        <v>7.2880000000000003</v>
+      </c>
+      <c r="E42" s="14">
+        <v>4.0810000000000004</v>
+      </c>
+      <c r="F42" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D43" s="14">
+        <v>4.43</v>
+      </c>
+      <c r="E43" s="14">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="F43" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="14">
+        <v>0.68500000000000005</v>
+      </c>
+      <c r="E44" s="14">
+        <v>1.909</v>
+      </c>
+      <c r="F44" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="D45" s="14">
+        <v>1.2E-2</v>
+      </c>
+      <c r="E45" s="14">
+        <v>3.8679999999999999</v>
+      </c>
+      <c r="F45" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C46" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" s="14">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="E46" s="14">
+        <v>4.0229999999999997</v>
+      </c>
+      <c r="F46" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C47" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D47" s="14">
+        <v>5.1580000000000004</v>
+      </c>
+      <c r="E47" s="14">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="F47" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" s="14">
+        <v>6.42</v>
+      </c>
+      <c r="E48" s="14">
+        <v>-7.4999999999999997E-2</v>
+      </c>
+      <c r="F48" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D49" s="14">
+        <v>6.0570000000000004</v>
+      </c>
+      <c r="E49" s="14">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="F49" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" s="14">
+        <v>11.798</v>
+      </c>
+      <c r="E50" s="14">
+        <v>1.026</v>
+      </c>
+      <c r="F50" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" s="14">
+        <v>7.125</v>
+      </c>
+      <c r="E51" s="14">
+        <v>2.6779999999999999</v>
+      </c>
+      <c r="F51" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D52" s="26">
+        <v>6.3810000000000002</v>
+      </c>
+      <c r="E52" s="26">
+        <v>0.3</v>
+      </c>
+      <c r="F52" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D53" s="2"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D55" s="2"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D56" s="2"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D58" s="2"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D59" s="2"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D60" s="2"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D61" s="2"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D62" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L109"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9503,1340 +10188,635 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" s="19" t="s">
         <v>73</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>69</v>
+        <v>4</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="D3" s="9">
-        <v>6.9089999999999998</v>
+        <v>37.226999999999997</v>
       </c>
       <c r="E3" s="10">
-        <v>3.8239999999999998</v>
+        <v>0.19</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D4" s="9">
-        <v>3.8069999999999999</v>
+        <v>4.3250000000000002</v>
       </c>
       <c r="E4" s="10">
-        <v>5.0570000000000004</v>
+        <v>1.5</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="D5" s="9">
-        <v>2.0910000000000002</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="E5" s="10">
-        <v>-4.2999999999999997E-2</v>
+        <v>2.843</v>
       </c>
       <c r="F5" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="13">
+        <v>3.7810000000000001</v>
+      </c>
+      <c r="E6" s="14">
+        <v>3.0150000000000001</v>
+      </c>
+      <c r="F6" s="23" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="9">
-        <v>0.217</v>
-      </c>
-      <c r="E6" s="10">
-        <v>0.496</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>71</v>
-      </c>
-    </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="9">
-        <v>0.08</v>
-      </c>
-      <c r="E7" s="10">
-        <v>1.7150000000000001</v>
-      </c>
-      <c r="F7" s="21" t="s">
+      <c r="A7" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="13">
+        <v>3.1930000000000001</v>
+      </c>
+      <c r="E7" s="14">
+        <v>-8.5000000000000006E-2</v>
+      </c>
+      <c r="F7" s="23" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="D8" s="13">
-        <v>11.439</v>
+        <v>0.502</v>
       </c>
       <c r="E8" s="14">
-        <v>1.946</v>
+        <v>1.1140000000000001</v>
       </c>
       <c r="F8" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="D9" s="13">
-        <v>2.5779999999999998</v>
+        <v>0.222</v>
       </c>
       <c r="E9" s="14">
-        <v>-0.08</v>
+        <v>3.141</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D10" s="13">
-        <v>1.9790000000000001</v>
+        <v>10.382999999999999</v>
       </c>
       <c r="E10" s="14">
-        <v>0.27200000000000002</v>
+        <v>0.315</v>
       </c>
       <c r="F10" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="D11" s="13">
-        <v>1.6990000000000001</v>
+        <v>4.657</v>
       </c>
       <c r="E11" s="14">
-        <v>0.625</v>
+        <v>-3.2000000000000001E-2</v>
       </c>
       <c r="F11" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B12" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>55</v>
+        <v>2</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="D12" s="13">
-        <v>-4.2999999999999997E-2</v>
+        <v>3.2490000000000001</v>
       </c>
       <c r="E12" s="14">
-        <v>0.67400000000000004</v>
+        <v>0.41299999999999998</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B13" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>47</v>
+        <v>2</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>69</v>
       </c>
       <c r="D13" s="13">
-        <v>5.6289999999999996</v>
+        <v>2.8809999999999998</v>
       </c>
       <c r="E13" s="14">
-        <v>0.67200000000000004</v>
+        <v>0.79900000000000004</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="D14" s="13">
-        <v>4.8849999999999998</v>
+        <v>2.3220000000000001</v>
       </c>
       <c r="E14" s="14">
-        <v>0.59499999999999997</v>
+        <v>1.8360000000000001</v>
       </c>
       <c r="F14" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="27">
-        <v>2.0409999999999999</v>
-      </c>
-      <c r="E15" s="26">
-        <v>-0.01</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>72</v>
-      </c>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="13">
+        <v>1.746</v>
+      </c>
+      <c r="E15" s="14">
+        <v>3.2669999999999999</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="13">
+        <v>1.663</v>
+      </c>
+      <c r="E16" s="14">
+        <v>1.405</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="13">
+        <v>-6.3E-2</v>
+      </c>
+      <c r="E17" s="14">
+        <v>5.4409999999999998</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="13">
+        <v>9.9130000000000003</v>
+      </c>
+      <c r="E18" s="14">
+        <v>0.114</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="27">
+        <v>2.0840000000000001</v>
+      </c>
+      <c r="E19" s="26">
+        <v>1.8779999999999999</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="6"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="31" t="s">
-        <v>75</v>
+      <c r="A34" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B35" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C35" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="E35" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="F35" s="19" t="s">
         <v>73</v>
-      </c>
-      <c r="D35" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E35" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="F35" s="19" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="D36" s="10">
-        <v>1.5409999999999999</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="E36" s="10">
-        <v>5.1840000000000002</v>
+        <v>0.11</v>
       </c>
       <c r="F36" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D37" s="14">
+        <v>1.133</v>
+      </c>
+      <c r="E37" s="14">
+        <v>1.4179999999999999</v>
+      </c>
+      <c r="F37" s="23" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="D37" s="10">
-        <v>5.2190000000000003</v>
-      </c>
-      <c r="E37" s="10">
-        <v>15.752000000000001</v>
-      </c>
-      <c r="F37" s="21" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D38" s="14">
+        <v>1.0629999999999999</v>
+      </c>
+      <c r="E38" s="14">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="F38" s="23" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D38" s="10">
-        <v>0.51100000000000001</v>
-      </c>
-      <c r="E38" s="10">
-        <v>3.339</v>
-      </c>
-      <c r="F38" s="21" t="s">
-        <v>71</v>
-      </c>
-    </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D39" s="10">
-        <v>1.542</v>
-      </c>
-      <c r="E39" s="10">
-        <v>5.8360000000000003</v>
-      </c>
-      <c r="F39" s="21" t="s">
+      <c r="A39" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="14">
+        <v>3.9510000000000001</v>
+      </c>
+      <c r="E39" s="14">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="F39" s="23" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D40" s="14">
-        <v>2.097</v>
+        <v>1.1970000000000001</v>
       </c>
       <c r="E40" s="14">
-        <v>2.1800000000000002</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="F40" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="D41" s="14">
-        <v>6.3730000000000002</v>
+        <v>1.1240000000000001</v>
       </c>
       <c r="E41" s="14">
-        <v>1.292</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="F41" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>68</v>
+        <v>4</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="D42" s="14">
-        <v>7.2880000000000003</v>
+        <v>2.3330000000000002</v>
       </c>
       <c r="E42" s="14">
-        <v>4.0810000000000004</v>
+        <v>-0.03</v>
       </c>
       <c r="F42" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D43" s="14">
-        <v>4.43</v>
+        <v>1.7250000000000001</v>
       </c>
       <c r="E43" s="14">
-        <v>0.17899999999999999</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="F43" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D44" s="14">
-        <v>0.68500000000000005</v>
+        <v>1.93</v>
       </c>
       <c r="E44" s="14">
-        <v>1.909</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="F44" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="D45" s="14">
-        <v>1.2E-2</v>
+        <v>1.8740000000000001</v>
       </c>
       <c r="E45" s="14">
-        <v>3.8679999999999999</v>
+        <v>0.23899999999999999</v>
       </c>
       <c r="F45" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D46" s="14">
-        <v>0.54500000000000004</v>
+        <v>3.3010000000000002</v>
       </c>
       <c r="E46" s="14">
-        <v>4.0229999999999997</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="F46" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="D47" s="14">
-        <v>5.1580000000000004</v>
+        <v>1.333</v>
       </c>
       <c r="E47" s="14">
-        <v>1.1060000000000001</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F47" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B48" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D48" s="14">
-        <v>6.42</v>
-      </c>
-      <c r="E48" s="14">
-        <v>-7.4999999999999997E-2</v>
-      </c>
-      <c r="F48" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B49" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D49" s="14">
-        <v>6.0570000000000004</v>
-      </c>
-      <c r="E49" s="14">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="F49" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D50" s="14">
-        <v>11.798</v>
-      </c>
-      <c r="E50" s="14">
-        <v>1.026</v>
-      </c>
-      <c r="F50" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="B51" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D51" s="14">
-        <v>7.125</v>
-      </c>
-      <c r="E51" s="14">
-        <v>2.6779999999999999</v>
-      </c>
-      <c r="F51" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="B52" s="25" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D52" s="26">
-        <v>6.3810000000000002</v>
-      </c>
-      <c r="E52" s="26">
-        <v>0.3</v>
-      </c>
-      <c r="F52" s="28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D53" s="2"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D54" s="2"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D55" s="2"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D56" s="2"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D57" s="2"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D58" s="2"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D59" s="2"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D62" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L109"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F64" sqref="F64"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="2" customWidth="1"/>
-    <col min="6" max="6" width="24.5703125" style="4" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
         <v>65</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D2" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="9">
-        <v>37.226999999999997</v>
-      </c>
-      <c r="E3" s="10">
-        <v>0.19</v>
-      </c>
-      <c r="F3" s="21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="9">
-        <v>4.3250000000000002</v>
-      </c>
-      <c r="E4" s="10">
-        <v>1.5</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="9">
-        <v>0.34499999999999997</v>
-      </c>
-      <c r="E5" s="10">
-        <v>2.843</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="13">
-        <v>3.7810000000000001</v>
-      </c>
-      <c r="E6" s="14">
-        <v>3.0150000000000001</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="13">
-        <v>3.1930000000000001</v>
-      </c>
-      <c r="E7" s="14">
-        <v>-8.5000000000000006E-2</v>
-      </c>
-      <c r="F7" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="13">
-        <v>0.502</v>
-      </c>
-      <c r="E8" s="14">
-        <v>1.1140000000000001</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="13">
-        <v>0.222</v>
-      </c>
-      <c r="E9" s="14">
-        <v>3.141</v>
-      </c>
-      <c r="F9" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="13">
-        <v>10.382999999999999</v>
-      </c>
-      <c r="E10" s="14">
-        <v>0.315</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="13">
-        <v>4.657</v>
-      </c>
-      <c r="E11" s="14">
-        <v>-3.2000000000000001E-2</v>
-      </c>
-      <c r="F11" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="13">
-        <v>3.2490000000000001</v>
-      </c>
-      <c r="E12" s="14">
-        <v>0.41299999999999998</v>
-      </c>
-      <c r="F12" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="13">
-        <v>2.8809999999999998</v>
-      </c>
-      <c r="E13" s="14">
-        <v>0.79900000000000004</v>
-      </c>
-      <c r="F13" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="13">
-        <v>2.3220000000000001</v>
-      </c>
-      <c r="E14" s="14">
-        <v>1.8360000000000001</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="13">
-        <v>1.746</v>
-      </c>
-      <c r="E15" s="14">
-        <v>3.2669999999999999</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="13">
-        <v>1.663</v>
-      </c>
-      <c r="E16" s="14">
-        <v>1.405</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="13">
-        <v>-6.3E-2</v>
-      </c>
-      <c r="E17" s="14">
-        <v>5.4409999999999998</v>
-      </c>
-      <c r="F17" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D18" s="13">
-        <v>9.9130000000000003</v>
-      </c>
-      <c r="E18" s="14">
-        <v>0.114</v>
-      </c>
-      <c r="F18" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B19" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="27">
-        <v>2.0840000000000001</v>
-      </c>
-      <c r="E19" s="26">
-        <v>1.8779999999999999</v>
-      </c>
-      <c r="F19" s="28" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C35" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E35" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="F35" s="19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" s="10">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="E36" s="10">
-        <v>0.11</v>
-      </c>
-      <c r="F36" s="21" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B37" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D37" s="14">
-        <v>1.133</v>
-      </c>
-      <c r="E37" s="14">
-        <v>1.4179999999999999</v>
-      </c>
-      <c r="F37" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D38" s="14">
-        <v>1.0629999999999999</v>
-      </c>
-      <c r="E38" s="14">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="F38" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D39" s="14">
-        <v>3.9510000000000001</v>
-      </c>
-      <c r="E39" s="14">
-        <v>0.13100000000000001</v>
-      </c>
-      <c r="F39" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" s="14">
-        <v>1.1970000000000001</v>
-      </c>
-      <c r="E40" s="14">
-        <v>-2.5000000000000001E-2</v>
-      </c>
-      <c r="F40" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="14">
-        <v>1.1240000000000001</v>
-      </c>
-      <c r="E41" s="14">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="F41" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B42" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D42" s="14">
-        <v>2.3330000000000002</v>
-      </c>
-      <c r="E42" s="14">
-        <v>-0.03</v>
-      </c>
-      <c r="F42" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B43" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" s="14">
-        <v>1.7250000000000001</v>
-      </c>
-      <c r="E43" s="14">
-        <v>-2.5000000000000001E-2</v>
-      </c>
-      <c r="F43" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B44" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D44" s="14">
-        <v>1.93</v>
-      </c>
-      <c r="E44" s="14">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="F44" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D45" s="14">
-        <v>1.8740000000000001</v>
-      </c>
-      <c r="E45" s="14">
-        <v>0.23899999999999999</v>
-      </c>
-      <c r="F45" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B46" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D46" s="14">
-        <v>3.3010000000000002</v>
-      </c>
-      <c r="E46" s="14">
-        <v>8.8999999999999996E-2</v>
-      </c>
-      <c r="F46" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="B47" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="14">
-        <v>1.333</v>
-      </c>
-      <c r="E47" s="14">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="F47" s="23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="22" t="s">
-        <v>66</v>
       </c>
       <c r="B48" s="11" t="s">
         <v>4</v>
@@ -10851,12 +10831,12 @@
         <v>0.21099999999999999</v>
       </c>
       <c r="F48" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B49" s="25" t="s">
         <v>1</v>
@@ -10871,7 +10851,7 @@
         <v>3.1E-2</v>
       </c>
       <c r="F49" s="28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>